<commit_message>
Update data analysis summary1.xlsx
</commit_message>
<xml_diff>
--- a/PHAS0052/data analysis summary1.xlsx
+++ b/PHAS0052/data analysis summary1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\const\Dropbox\My PC (LAPTOP-QC4FGQ25)\Downloads\PHAS0052\PHAS0052\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantinos\Documents\GitHub\LLMs-in-Physics-Education\PHAS0052\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12F2BAA-BA83-4BB8-9B5C-63EA7723B762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB3047C-748E-445F-AE2C-86BBE2EEB3B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5956CF43-8F1D-446F-946F-9D1ED0AF9F45}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5956CF43-8F1D-446F-946F-9D1ED0AF9F45}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -175,6 +175,30 @@
   </si>
   <si>
     <t>Grok 3</t>
+  </si>
+  <si>
+    <t>R_raw_cm_without</t>
+  </si>
+  <si>
+    <t>R_raw_cm_with</t>
+  </si>
+  <si>
+    <t>R_raw_em_without</t>
+  </si>
+  <si>
+    <t>R_raw_em_with</t>
+  </si>
+  <si>
+    <t>R_raw_qm_without</t>
+  </si>
+  <si>
+    <t>R_raw_qm_with</t>
+  </si>
+  <si>
+    <t>R_raw_without</t>
+  </si>
+  <si>
+    <t>R_raw_with</t>
   </si>
 </sst>
 </file>
@@ -635,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A4CE3-2772-40EF-AB98-CAF254C6F39D}">
-  <dimension ref="A1:AO23"/>
+  <dimension ref="A1:AW23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AM9" sqref="AM9"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z1" sqref="Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -678,7 +702,7 @@
     <col min="42" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="4" customFormat="1" ht="15">
+    <row r="1" spans="1:49" s="4" customFormat="1" ht="15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -802,8 +826,32 @@
       <c r="AO1" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="AP1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AT1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AW1" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:41" s="4" customFormat="1" ht="15.75">
+    <row r="2" spans="1:49" s="4" customFormat="1" ht="15.75">
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
@@ -927,8 +975,32 @@
       <c r="AO2" s="8">
         <v>3.16308243727598</v>
       </c>
+      <c r="AP2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="AQ2" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="AR2" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="AS2" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="AT2" s="2">
+        <v>0.92</v>
+      </c>
+      <c r="AU2" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="AV2" s="4">
+        <v>0.77</v>
+      </c>
+      <c r="AW2" s="2">
+        <v>0.76</v>
+      </c>
     </row>
-    <row r="3" spans="1:41" s="4" customFormat="1" ht="15">
+    <row r="3" spans="1:49" s="4" customFormat="1" ht="15.75">
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
@@ -1052,8 +1124,32 @@
       <c r="AO3" s="8">
         <v>3.8346134152585698</v>
       </c>
+      <c r="AP3" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="AQ3" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="AR3" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="AS3" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="AT3" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="AU3" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="AV3" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="AW3" s="2">
+        <v>0.81</v>
+      </c>
     </row>
-    <row r="4" spans="1:41" s="4" customFormat="1" ht="15">
+    <row r="4" spans="1:49" s="4" customFormat="1" ht="15.75">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
@@ -1177,8 +1273,32 @@
       <c r="AO4" s="8">
         <v>3.8866700802184599</v>
       </c>
+      <c r="AP4" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="AQ4" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="AR4" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="AS4" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="AT4" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="AU4" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="AV4" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AW4" s="2">
+        <v>0.67</v>
+      </c>
     </row>
-    <row r="5" spans="1:41" s="4" customFormat="1" ht="15">
+    <row r="5" spans="1:49" s="4" customFormat="1" ht="15.75">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
@@ -1302,8 +1422,32 @@
       <c r="AO5" s="8">
         <v>5.2775217613927197</v>
       </c>
+      <c r="AP5" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="AQ5" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="AR5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AS5" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AT5" s="2">
+        <v>0.94</v>
+      </c>
+      <c r="AU5" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="AV5" s="2">
+        <v>0.73</v>
+      </c>
+      <c r="AW5" s="2">
+        <v>0.55000000000000004</v>
+      </c>
     </row>
-    <row r="6" spans="1:41" s="4" customFormat="1" ht="15">
+    <row r="6" spans="1:49" s="4" customFormat="1" ht="15.75">
       <c r="A6" s="4" t="s">
         <v>45</v>
       </c>
@@ -1426,6 +1570,30 @@
       </c>
       <c r="AO6" s="8">
         <v>3.0349520182960301</v>
+      </c>
+      <c r="AP6" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="AQ6" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="AR6" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="AS6" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AT6" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="AU6" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="AV6" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="AW6" s="2">
+        <v>0.83</v>
       </c>
     </row>
     <row r="23" spans="21:21" ht="15.75">

</xml_diff>